<commit_message>
Deploying to gh-pages from @ eurovibes/dc_shield@b4b83e717ff7e5e7c1d952959d342fe6ca09a09f 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/dc_shield-bom_0.2.xlsx
+++ b/Fabrication/BoM/dc_shield-bom_0.2.xlsx
@@ -503,25 +503,25 @@
     <t>U105 U106</t>
   </si>
   <si>
-    <t>ACS712xLCTR-05B</t>
-  </si>
-  <si>
-    <t>ACS712ELCTR-05B</t>
-  </si>
-  <si>
-    <t>ACS712ELCTR-05B-T</t>
+    <t>ACS712xLCTR-20A</t>
+  </si>
+  <si>
+    <t>ACS712ELCTR-20A</t>
+  </si>
+  <si>
+    <t>ACS712ELCTR-20A-T</t>
   </si>
   <si>
     <t>Allegro MicroSystems, LLC</t>
   </si>
   <si>
-    <t>https://jlcpcb.com/partdetail/45473-ACS712ELCTR_05BT/C44471</t>
+    <t>https://jlcpcb.com/partdetail/11225-ACS712ELCTR_20AT/C10681</t>
   </si>
   <si>
     <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
-    <t>±5A Bidirectional Hall-Effect Current Sensor, +5.0V supply, 185mV/A, SOIC-8</t>
+    <t>±20A Bidirectional Hall-Effect Current Sensor, +5.0V supply, 100mV/A, SOIC-8</t>
   </si>
   <si>
     <t>22</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/dc_shield@f5ff49c75f3326117b95796ae41c3fb7995dba14 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/dc_shield-bom_0.2.xlsx
+++ b/Fabrication/BoM/dc_shield-bom_0.2.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="206">
   <si>
     <t>Row</t>
   </si>
@@ -98,31 +98,34 @@
     <t>22 nF</t>
   </si>
   <si>
-    <t>CC0603KRX7R9BB223</t>
+    <t>CL10B223KB8NNNC</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/21834-CL10B223KB8NNNC/C21122</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>C109 C112 C117 C118 C119 C120</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB104</t>
   </si>
   <si>
     <t>YAGEO</t>
   </si>
   <si>
-    <t>https://jlcpcb.com/partdetail/Yageo-CC0603KRX7R9BB223/C106222</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>C109 C112 C117 C118</t>
-  </si>
-  <si>
-    <t>100 nF</t>
-  </si>
-  <si>
-    <t>CL10B104KB8NNNC</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/1943-CL10B104KB8NNNC/C1591</t>
+    <t>https://jlcpcb.com/partdetail/Yageo-CC0603KRX7R9BB104/C14663</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
   <si>
     <t>C101</t>
@@ -131,13 +134,10 @@
     <t>1 µF</t>
   </si>
   <si>
-    <t>0603F105M500NT</t>
-  </si>
-  <si>
-    <t>FH (Guangdong Fenghua Advanced Tech)</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/109562-0603F105M500NT/C108343</t>
+    <t>CL10A105KB8NNNC</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/16531-CL10A105KB8NNNC/C15849</t>
   </si>
   <si>
     <t>5</t>
@@ -149,21 +149,15 @@
     <t>10 µF</t>
   </si>
   <si>
-    <t>C3216X5R1H106KT000N</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Tdk-C3216X5R1H106KT000N/C329928</t>
+    <t>CL31A106KBHNNNE</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/14236-CL31A106KBHNNNE/C13585</t>
   </si>
   <si>
     <t>C_1206_3216Metric</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>C107 C110</t>
   </si>
   <si>
@@ -173,13 +167,13 @@
     <t>330 µF</t>
   </si>
   <si>
-    <t>CS1H331M-CRG10</t>
-  </si>
-  <si>
-    <t>ROQANG</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Roqang-CS1H331MCRG10/C5162354</t>
+    <t>VZT331M1HTR-1010</t>
+  </si>
+  <si>
+    <t>Lelon</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/Lelon-VZT331M1HTR1010/C249985</t>
   </si>
   <si>
     <t>CP_Elec_10x10.5</t>
@@ -440,16 +434,16 @@
     <t>R</t>
   </si>
   <si>
-    <t>1.1 Ω</t>
-  </si>
-  <si>
-    <t>WR12W1R10FTL</t>
-  </si>
-  <si>
-    <t>Walsin Tech Corp</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/Walsin_TechCorp-WR12W1R10FTL/C168518</t>
+    <t>1 Ω</t>
+  </si>
+  <si>
+    <t>1206W4F100KT5E</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/18616-1206W4F100KT5E/C17928</t>
   </si>
   <si>
     <t>R_1206_3216Metric</t>
@@ -470,9 +464,6 @@
     <t>0402WGF2001TCE</t>
   </si>
   <si>
-    <t>UNI-ROYAL(Uniroyal Elec)</t>
-  </si>
-  <si>
     <t>https://jlcpcb.com/partdetail/4516-0402WGF2001TCE/C4109</t>
   </si>
   <si>
@@ -488,13 +479,10 @@
     <t>10 kΩ</t>
   </si>
   <si>
-    <t>AR02DTC1002</t>
-  </si>
-  <si>
-    <t>Viking Tech</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/VikingTech-AR02DTC1002/C319934</t>
+    <t>0402WGF1002TCE</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/26487-0402WGF1002TCE/C25744</t>
   </si>
   <si>
     <t>21</t>
@@ -800,8 +788,8 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1218279</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:colOff>1084929</xdr:colOff>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>58841</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1136,11 +1124,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
     <col min="9" max="9" width="60.7109375" customWidth="1"/>
@@ -1151,7 +1139,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1165,13 +1153,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F2" s="3">
         <v>24</v>
@@ -1179,41 +1167,41 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F3" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F4" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1221,16 +1209,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F6" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1309,7 +1297,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1">
+    <row r="10" spans="1:12">
       <c r="A10" s="8" t="s">
         <v>23</v>
       </c>
@@ -1326,7 +1314,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>18</v>
@@ -1335,7 +1323,7 @@
         <v>19</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>21</v>
@@ -1344,27 +1332,27 @@
         <v>22</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>18</v>
@@ -1382,27 +1370,27 @@
         <v>22</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>18</v>
@@ -1423,7 +1411,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
+    <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
@@ -1440,7 +1428,7 @@
         <v>43</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>18</v>
@@ -1449,10 +1437,10 @@
         <v>19</v>
       </c>
       <c r="I13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>22</v>
@@ -1463,22 +1451,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="F14" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>18</v>
@@ -1487,13 +1475,13 @@
         <v>19</v>
       </c>
       <c r="I14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>23</v>
@@ -1501,22 +1489,22 @@
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>18</v>
@@ -1525,13 +1513,13 @@
         <v>19</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="J15" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>23</v>
@@ -1539,22 +1527,22 @@
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="D16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>66</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>18</v>
@@ -1563,13 +1551,13 @@
         <v>19</v>
       </c>
       <c r="I16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>12</v>
@@ -1577,22 +1565,22 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E17" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>18</v>
@@ -1601,13 +1589,13 @@
         <v>19</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>12</v>
@@ -1615,22 +1603,22 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="E18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>82</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>18</v>
@@ -1639,13 +1627,13 @@
         <v>19</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>12</v>
@@ -1653,37 +1641,37 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="E19" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="F19" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="J19" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>12</v>
@@ -1691,37 +1679,37 @@
     </row>
     <row r="20" spans="1:12" ht="30" customHeight="1">
       <c r="A20" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="E20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="K20" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>12</v>
@@ -1729,37 +1717,37 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="E21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="K21" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>23</v>
@@ -1767,75 +1755,75 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="F22" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="G22" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" s="10" t="s">
+      <c r="J22" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="K22" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="J22" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="L22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="F23" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="H23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="K23" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>12</v>
@@ -1843,16 +1831,16 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>128</v>
-      </c>
       <c r="D24" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>19</v>
@@ -1870,33 +1858,33 @@
         <v>19</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K24" s="10" t="s">
         <v>19</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="F25" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>18</v>
@@ -1905,36 +1893,36 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K25" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="K25" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="30" customHeight="1">
+    <row r="26" spans="1:12">
       <c r="A26" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="E26" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="F26" s="10" t="s">
         <v>140</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>142</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>18</v>
@@ -1943,13 +1931,13 @@
         <v>19</v>
       </c>
       <c r="I26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>12</v>
@@ -1957,22 +1945,22 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="E27" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>149</v>
-      </c>
       <c r="F27" s="7" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>18</v>
@@ -1981,13 +1969,13 @@
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>23</v>
@@ -1995,22 +1983,22 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>156</v>
-      </c>
       <c r="F28" s="10" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>18</v>
@@ -2019,36 +2007,36 @@
         <v>19</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="F29" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>18</v>
@@ -2057,13 +2045,13 @@
         <v>19</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K29" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>23</v>
@@ -2071,22 +2059,22 @@
     </row>
     <row r="30" spans="1:12" ht="30" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F30" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>18</v>
@@ -2095,13 +2083,13 @@
         <v>19</v>
       </c>
       <c r="I30" s="10" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>12</v>
@@ -2109,22 +2097,22 @@
     </row>
     <row r="31" spans="1:12" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>18</v>
@@ -2133,10 +2121,10 @@
         <v>19</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K31" s="7" t="s">
         <v>19</v>
@@ -2147,37 +2135,37 @@
     </row>
     <row r="32" spans="1:12" ht="30" customHeight="1">
       <c r="A32" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="G32" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H32" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="I32" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="J32" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="F32" s="10" t="s">
+      <c r="K32" s="10" t="s">
         <v>185</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="K32" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="L32" s="8" t="s">
         <v>12</v>
@@ -2232,22 +2220,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>